<commit_message>
Memasukkan total usage ke dalam draft cac
</commit_message>
<xml_diff>
--- a/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
+++ b/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sep 22" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -185,9 +185,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -590,10 +590,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -614,62 +614,62 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,10 +678,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -693,7 +693,7 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -702,7 +702,7 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -710,7 +710,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -719,16 +719,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -740,38 +740,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -781,33 +781,33 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -823,7 +823,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1170,7 +1170,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1363,7 +1363,7 @@
         <v>100000000</v>
       </c>
       <c r="I7" s="14">
-        <v>20000000</v>
+        <v>18888888.888888799</v>
       </c>
       <c r="J7" s="15">
         <v>80000000</v>
@@ -10939,6 +10939,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9F1EEA8DBA4264CBE4017FBB2A43667" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3afbaf582f20c73f6f3f1e0d866ff50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6a9967f0-2ede-4e66-b25a-34d1858201b8" xmlns:ns4="53d79d5c-2d4a-4ddc-9289-8854791c3284" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77f62bdf32cf1fc9992a2b564b6a700a" ns3:_="" ns4:_="">
     <xsd:import namespace="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
@@ -11121,22 +11136,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA88657D-EE78-434B-B0D7-6D51BE53B86F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
+    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AF2971-DAA2-4BDF-8276-EAC890BDDD44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16825FA-1465-4BA1-907C-AE62FD5E9FFC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11153,29 +11178,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AF2971-DAA2-4BDF-8276-EAC890BDDD44}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA88657D-EE78-434B-B0D7-6D51BE53B86F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
-    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add input cac sequence to main sequence
</commit_message>
<xml_diff>
--- a/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
+++ b/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICStar Hackathon\final-project\project\Final Project\Data Project ICStar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sep 22" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -183,11 +188,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -590,10 +595,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -614,62 +619,62 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,10 +683,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -693,7 +698,7 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -702,7 +707,7 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -710,7 +715,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -719,16 +724,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -740,38 +745,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -781,33 +786,33 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -823,7 +828,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1170,7 +1175,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
save document result into result folder
</commit_message>
<xml_diff>
--- a/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
+++ b/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
@@ -10944,21 +10944,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9F1EEA8DBA4264CBE4017FBB2A43667" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3afbaf582f20c73f6f3f1e0d866ff50">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6a9967f0-2ede-4e66-b25a-34d1858201b8" xmlns:ns4="53d79d5c-2d4a-4ddc-9289-8854791c3284" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77f62bdf32cf1fc9992a2b564b6a700a" ns3:_="" ns4:_="">
     <xsd:import namespace="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
@@ -11141,32 +11126,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA88657D-EE78-434B-B0D7-6D51BE53B86F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
-    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AF2971-DAA2-4BDF-8276-EAC890BDDD44}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16825FA-1465-4BA1-907C-AE62FD5E9FFC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11183,4 +11158,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09AF2971-DAA2-4BDF-8276-EAC890BDDD44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA88657D-EE78-434B-B0D7-6D51BE53B86F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
+    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
menambahkan form dan memperbaiki path file/folder
</commit_message>
<xml_diff>
--- a/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
+++ b/Final Project/Data Project ICStar/DRAFT CAC UNTUK HACKATHON.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ICStar Hackathon\final-project\project\Final Project\Data Project ICStar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sep 22" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -188,11 +183,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -595,10 +590,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,62 +614,62 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -683,10 +678,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -698,7 +693,7 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,7 +702,7 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,7 +710,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,16 +719,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -745,38 +740,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="21" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -786,33 +781,33 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="24" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,7 +823,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1175,7 +1170,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1187,7 +1182,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="80" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -1379,8 +1374,8 @@
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="17">
-        <f>L8</f>
-        <v>60000000</v>
+        <f>H7-I7-K7</f>
+        <v>61111111.111111194</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="18"/>
@@ -1619,7 +1614,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:32" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
@@ -11144,16 +11139,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA88657D-EE78-434B-B0D7-6D51BE53B86F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6a9967f0-2ede-4e66-b25a-34d1858201b8"/>
-    <ds:schemaRef ds:uri="53d79d5c-2d4a-4ddc-9289-8854791c3284"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>